<commit_message>
GoodInfo_v2 - 2021.12.08 完成
</commit_message>
<xml_diff>
--- a/Filter_20211208.xlsx
+++ b/Filter_20211208.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayWu\OneDrive - AAEON Technology\_OLD\Documents\Python\GoodInfo_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\GoodInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_7E8059E53D79F080A6D05B09F3D2F4F3B881A88D" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A976F3A6-DB91-4212-B5B0-8519296FD30B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18816" windowHeight="7968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18816" windowHeight="7968"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="146">
   <si>
     <t>代號</t>
   </si>
@@ -454,12 +453,36 @@
   </si>
   <si>
     <t>聯邦銀</t>
+  </si>
+  <si>
+    <t>光頡</t>
+  </si>
+  <si>
+    <t>新美齊</t>
+  </si>
+  <si>
+    <t>協益</t>
+  </si>
+  <si>
+    <t>東和鋼鐵</t>
+  </si>
+  <si>
+    <t>聯電</t>
+  </si>
+  <si>
+    <t>浩鑫</t>
+  </si>
+  <si>
+    <t>英濟</t>
+  </si>
+  <si>
+    <t>錸寶</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -862,11 +885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:B94"/>
+      <selection activeCell="A102" sqref="A102:B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1909,6 +1932,70 @@
       </c>
       <c r="B94" s="2" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <v>3624</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <v>2442</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>5356</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>2303</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>2405</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>3294</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>8104</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1922,12 +2009,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2140,15 +2224,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81046D84-71BA-4494-97FE-ABE61A155419}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1E403E-48E0-45A5-8A6B-E1BE8411359D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2173,18 +2269,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC1E403E-48E0-45A5-8A6B-E1BE8411359D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81046D84-71BA-4494-97FE-ABE61A155419}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>